<commit_message>
Added some new graphs!
</commit_message>
<xml_diff>
--- a/Track two dialogue database.xlsx
+++ b/Track two dialogue database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berna\Documents\R\track-two-dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF7C798-2BAB-48A0-A434-598A6AF2DFD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DF4023-68D9-412E-8AC4-ABC330F87D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{862A2EDB-63C4-4B07-B101-E010855B3AF9}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">End Date </t>
   </si>
   <si>
-    <t>CISAC Russia Dialogue</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elbe group </t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Pugwash</t>
   </si>
   <si>
-    <t xml:space="preserve">Dartmouth Confernece </t>
-  </si>
-  <si>
     <t>NAS CISAC</t>
   </si>
   <si>
@@ -332,9 +326,6 @@
     <t xml:space="preserve">NDU dialogue </t>
   </si>
   <si>
-    <t xml:space="preserve">CEIP workign group on U.S.-Russia relations </t>
-  </si>
-  <si>
     <t xml:space="preserve">Nixon center project </t>
   </si>
   <si>
@@ -414,6 +405,15 @@
   </si>
   <si>
     <t>ACONA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEIP working group on U.S.-Russia relations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dartmouth Conference </t>
+  </si>
+  <si>
+    <t>National Academy of Sciences Committee on International Security and Arms Control Russia Dialogue</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB829A12-B58E-43FC-8FC0-B2D51D61C2DC}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,13 +819,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -834,27 +834,27 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1957</v>
@@ -868,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1960</v>
@@ -882,13 +882,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>1980</v>
@@ -897,24 +897,24 @@
         <v>2020</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>2001</v>
@@ -923,21 +923,21 @@
         <v>2002</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>2001</v>
@@ -946,27 +946,27 @@
         <v>2002</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>2001</v>
@@ -975,24 +975,24 @@
         <v>2005</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>2001</v>
@@ -1001,18 +1001,18 @@
         <v>2001</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>1980</v>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>2001</v>
@@ -1038,21 +1038,21 @@
         <v>2001</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5">
         <v>2007</v>
@@ -1061,27 +1061,27 @@
         <v>2008</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5">
         <v>2008</v>
@@ -1090,27 +1090,27 @@
         <v>2008</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="5">
         <v>2008</v>
@@ -1119,25 +1119,25 @@
         <v>2008</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>2010</v>
@@ -1146,18 +1146,18 @@
         <v>2020</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>2010</v>
@@ -1166,18 +1166,18 @@
         <v>2014</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>2012</v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>2013</v>
@@ -1203,18 +1203,18 @@
         <v>2020</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>2016</v>
@@ -1223,18 +1223,18 @@
         <v>2017</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>2016</v>
@@ -1243,18 +1243,18 @@
         <v>2017</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>2017</v>
@@ -1263,21 +1263,21 @@
         <v>2017</v>
       </c>
       <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
         <v>38</v>
-      </c>
-      <c r="I20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="5">
         <v>2017</v>
@@ -1286,20 +1286,20 @@
         <v>2020</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="5">
         <v>2019</v>
@@ -1308,23 +1308,23 @@
         <v>2019</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="5">
         <v>1996</v>
@@ -1333,27 +1333,27 @@
         <v>2002</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" t="s">
         <v>56</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>57</v>
-      </c>
-      <c r="I23" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="5">
         <v>1996</v>
@@ -1362,24 +1362,24 @@
         <v>2000</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" t="s">
         <v>61</v>
-      </c>
-      <c r="H24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="5">
         <v>2000</v>
@@ -1388,21 +1388,21 @@
         <v>2002</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5">
         <v>1999</v>
@@ -1411,18 +1411,18 @@
         <v>2020</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="5">
         <v>2002</v>
@@ -1431,24 +1431,24 @@
         <v>2004</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="5">
         <v>1984</v>
@@ -1457,18 +1457,18 @@
         <v>2020</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" s="5">
         <v>1982</v>
@@ -1477,18 +1477,18 @@
         <v>2020</v>
       </c>
       <c r="I29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="5">
         <v>1987</v>
@@ -1497,18 +1497,18 @@
         <v>1992</v>
       </c>
       <c r="I30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="5">
         <v>1990</v>
@@ -1517,21 +1517,21 @@
         <v>1992</v>
       </c>
       <c r="F31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" t="s">
         <v>76</v>
-      </c>
-      <c r="I31" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5">
         <v>1990</v>
@@ -1540,18 +1540,18 @@
         <v>1990</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="5">
         <v>1990</v>
@@ -1560,24 +1560,24 @@
         <v>1991</v>
       </c>
       <c r="F33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" t="s">
         <v>81</v>
-      </c>
-      <c r="G33" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>2005</v>
@@ -1586,24 +1586,24 @@
         <v>2020</v>
       </c>
       <c r="F34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" t="s">
         <v>84</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>85</v>
-      </c>
-      <c r="I34" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>2010</v>
@@ -1612,18 +1612,18 @@
         <v>2020</v>
       </c>
       <c r="F35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36">
         <v>2007</v>
@@ -1634,16 +1634,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="E37">
         <v>2014</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <v>2019</v>

</xml_diff>

<commit_message>
Made some new graphs!
</commit_message>
<xml_diff>
--- a/Track two dialogue database.xlsx
+++ b/Track two dialogue database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berna\Documents\R\track-two-dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DF4023-68D9-412E-8AC4-ABC330F87D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68FF531-34FF-4F5B-AC02-14B70424BE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{862A2EDB-63C4-4B07-B101-E010855B3AF9}"/>
+    <workbookView xWindow="9132" yWindow="2124" windowWidth="10356" windowHeight="8976" xr2:uid="{862A2EDB-63C4-4B07-B101-E010855B3AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB829A12-B58E-43FC-8FC0-B2D51D61C2DC}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>